<commit_message>
新文件的加入 Signed-off-by: gaoxe <648789030@qq,com>
</commit_message>
<xml_diff>
--- a/高小恩/工作中待解决的问题.xlsx
+++ b/高小恩/工作中待解决的问题.xlsx
@@ -10,13 +10,14 @@
     <sheet name="erLang学习" sheetId="2" r:id="rId1"/>
     <sheet name="每日计划" sheetId="3" r:id="rId2"/>
     <sheet name="周计划" sheetId="4" r:id="rId3"/>
+    <sheet name="做事准则" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
   <si>
     <t>遇到的问题</t>
   </si>
@@ -113,10 +114,58 @@
     <t>待做事项</t>
   </si>
   <si>
+    <t>执行情况</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
     <t>1.看完《erlang程序设计》6,7,8,9,10五章内容</t>
   </si>
   <si>
+    <t>完成</t>
+  </si>
+  <si>
+    <t>语法确实比较奇怪，特别是“，”,";","."的用法需要特别注意一下</t>
+  </si>
+  <si>
     <t>2.继续熟悉《erlang程序设计》第22,23章，构思聊天服务器的设计</t>
+  </si>
+  <si>
+    <t>22章完，23章未看，初步觉得，22章还是挺有难度的，跟着书上的代码进行编程，调试起来还是挺难的。聊天服务器的设计，应该是和12,13,14章关系比较密切，今天就主要看这三张的内容</t>
+  </si>
+  <si>
+    <t>在做22章练习的时候，发现如果执行的有一个错误，则后续的都执行不下去，也就是说这个进程算是crash掉了。</t>
+  </si>
+  <si>
+    <t>1.看完《erlang程序设计》11,12,13,14章内容</t>
+  </si>
+  <si>
+    <t>看完了，内容还需要再过一下</t>
+  </si>
+  <si>
+    <t>2.初步完成聊天服务器的基础设计</t>
+  </si>
+  <si>
+    <t>网上找到一段代码，关于聊天发消息的部分</t>
+  </si>
+  <si>
+    <t>有很多地方都很深，看不懂</t>
+  </si>
+  <si>
+    <t>3.看一下志江之前提供的网页，关于erlang编程的内容</t>
+  </si>
+  <si>
+    <t>看了一下初级版的日志教程，还是比较生疏</t>
+  </si>
+  <si>
+    <t>文档从入门开始讲起，内容相对比较生疏</t>
+  </si>
+  <si>
+    <t>1.看完《erlang程序设计》19,21,23三章</t>
+  </si>
+  <si>
+    <t>2.正式开发聊天服务器的功能，第一步，写需求 第二步 开发功能 第三部 测试</t>
   </si>
   <si>
     <t>1.erlang程序设计 看完</t>
@@ -126,6 +175,24 @@
 基础要求1 模块包括 ：登陆，验证，创建房间，关闭房间，默认第一个进去是管理员，管理员权限可以转移。
 进阶要求2 实现一个高性能的聊天服务器，写自动登陆客户端，压测在线最高能到多少。最好使用linux来压，win下有连接数限制。
 </t>
+  </si>
+  <si>
+    <t>做事的军规：</t>
+  </si>
+  <si>
+    <t>1.不要怕麻烦，所有的问题都想清楚，搞明白</t>
+  </si>
+  <si>
+    <t>2.不要怕麻烦，做完的功能，反复检查代码，反复测试，特别是测试配置表的功能是否正常</t>
+  </si>
+  <si>
+    <t>3.不要怕麻烦，对任何一个异常情况都要搞清楚，不要放过任何一处异常情况</t>
+  </si>
+  <si>
+    <t>4.不要怕担责任，凡是和自己相关的都积极查找问题，不是自己的，也要积极配合查找问题所在</t>
+  </si>
+  <si>
+    <t>5.坦然接受任何的结果，有问题就解决，不逃避，不忌讳，放松心情</t>
   </si>
 </sst>
 </file>
@@ -138,9 +205,17 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
-    <font>
-      <sz val="11"/>
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -485,7 +560,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -503,6 +578,32 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -614,10 +715,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -626,144 +727,162 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -1128,104 +1247,104 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="19.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="19.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="52.75" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32.875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.375" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" spans="1:6">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="9" customFormat="1" spans="1:6">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" ht="108" spans="1:6">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" ht="54" spans="1:6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" ht="67.5" spans="1:6">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" ht="121.5" spans="1:6">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -1236,44 +1355,120 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="1"/>
-    <col min="2" max="2" width="29.125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="11.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26.125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" ht="27" spans="1:2">
-      <c r="A2" s="2">
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" ht="40.5" spans="1:4">
+      <c r="A2" s="6">
         <v>20180507</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" ht="40.5" spans="1:2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" ht="145" customHeight="1" spans="1:4">
+      <c r="A3" s="6"/>
+      <c r="B3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" ht="27" spans="1:4">
+      <c r="A4" s="6">
+        <v>20180508</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" ht="27" spans="1:4">
+      <c r="A5" s="6"/>
+      <c r="B5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" ht="27" spans="1:4">
+      <c r="A6" s="6"/>
+      <c r="B6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" ht="27" spans="1:4">
+      <c r="A7" s="7">
+        <v>20180509</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" ht="40.5" spans="1:4">
+      <c r="A8" s="8"/>
+      <c r="B8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1286,7 +1481,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
@@ -1296,25 +1491,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" ht="29" customHeight="1" spans="1:2">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>20180507</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" ht="94.5" spans="1:2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1" t="s">
-        <v>28</v>
+      <c r="A3" s="4"/>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1324,4 +1519,55 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelRow="5"/>
+  <cols>
+    <col min="1" max="1" width="59.375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
增加了舞动的游戏代码和其他人的代码 Signed-off-by: gaoxe <648789030@qq,com>
</commit_message>
<xml_diff>
--- a/高小恩/工作中待解决的问题.xlsx
+++ b/高小恩/工作中待解决的问题.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050" tabRatio="652"/>
+    <workbookView windowWidth="28695" windowHeight="13050" tabRatio="652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="erLang学习" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70">
   <si>
     <t>遇到的问题</t>
   </si>
@@ -174,6 +174,42 @@
     <t>功能做完了，需要实际的再次测试</t>
   </si>
   <si>
+    <t>1.查看上周的代码，增加对代码覆盖率的使用</t>
+  </si>
+  <si>
+    <t>2.增加对进程的监控和挂掉重启</t>
+  </si>
+  <si>
+    <t>3.进行功能的压力测试</t>
+  </si>
+  <si>
+    <t>4.测试所有的活动功能是否正常运行，如果有异常，就修复</t>
+  </si>
+  <si>
+    <t>测试了一下，包括所有的运营活动和累充活动，发现有一个客户端显示的问题，功能不影响，是在跨天的时候出现的</t>
+  </si>
+  <si>
+    <t>1.查看其他人写的代码，关于聊天室功能</t>
+  </si>
+  <si>
+    <t>其中有看到，高伟的代码中有一个代码覆盖率的调试，使用的是rebar方法，这个需要自己实际的验证一下，怎么去用这个。代码覆盖率的验证很重要，能够避免很多的bug出现和奔溃</t>
+  </si>
+  <si>
+    <t>2.学习阅读舞动的服务器代码，了解整体结构设计</t>
+  </si>
+  <si>
+    <t>编译舞动代码，启动舞动服务器，游戏可以正常跑流程。查看整体的代码结构矿建</t>
+  </si>
+  <si>
+    <t>3.如有时间，做一下自己的服务器压测</t>
+  </si>
+  <si>
+    <t>4.OA申请问题处理并解决</t>
+  </si>
+  <si>
+    <t>5.苍之纪元 游戏的熟悉，装备物品模块</t>
+  </si>
+  <si>
     <t>检测</t>
   </si>
   <si>
@@ -190,6 +226,12 @@
   </si>
   <si>
     <t>基本要求已实现，需要完善功能设计。1.增加如果玩家没有登录名，就不能有任何操作 2.玩家可以退出房间操作 3.压力测试，测试最高在线人数</t>
+  </si>
+  <si>
+    <t>1.修改上周的连续，增加代码检测和挂掉重启功能</t>
+  </si>
+  <si>
+    <t>2.熟悉新的项目代码</t>
   </si>
   <si>
     <t>做事的军规：</t>
@@ -215,10 +257,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -246,6 +288,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -253,23 +303,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -282,14 +334,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,9 +349,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -311,6 +371,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -320,54 +388,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -380,6 +408,20 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -390,6 +432,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -402,13 +468,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,6 +480,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -438,6 +546,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -450,19 +594,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,104 +616,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -599,56 +641,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -660,41 +652,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,6 +679,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -730,10 +746,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -745,134 +761,134 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -882,22 +898,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -965,6 +975,95 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>618490</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10058400" y="5260975"/>
+          <a:ext cx="4161790" cy="1679575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>561340</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1619250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4781550" y="5280025"/>
+          <a:ext cx="5266690" cy="1609725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1256,39 +1355,39 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="19.125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="52.75" style="3" customWidth="1"/>
-    <col min="3" max="3" width="32.875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="26.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.375" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="19.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="52.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" spans="1:6">
-      <c r="A1" s="10" t="s">
+    <row r="1" s="7" customFormat="1" spans="1:6">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1367,19 +1466,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="11.375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="26.125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="11.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1459,7 +1558,7 @@
       </c>
     </row>
     <row r="7" ht="27" spans="1:4">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>20180509</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1473,7 +1572,7 @@
       </c>
     </row>
     <row r="8" ht="40.5" spans="1:4">
-      <c r="A8" s="8"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="5" t="s">
         <v>43</v>
       </c>
@@ -1484,27 +1583,112 @@
         <v>44</v>
       </c>
     </row>
+    <row r="9" ht="27" spans="1:4">
+      <c r="A9" s="4">
+        <v>20180514</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" ht="27" spans="1:4">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" ht="130" customHeight="1" spans="1:4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" ht="81" spans="1:4">
+      <c r="A13" s="4">
+        <v>20180516</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" ht="40.5" spans="1:4">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" ht="27" spans="1:4">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" ht="27" spans="1:4">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="12.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="46.75" style="2" customWidth="1"/>
@@ -1519,8 +1703,8 @@
       <c r="B1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>45</v>
+      <c r="C1" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" ht="29" customHeight="1" spans="1:3">
@@ -1528,24 +1712,41 @@
         <v>20180507</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" ht="94.5" spans="1:3">
       <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4">
+        <v>20180514</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1558,7 +1759,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelRow="5"/>
@@ -1569,32 +1770,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>